<commit_message>
Added 5% chance to roll 4
</commit_message>
<xml_diff>
--- a/Tile-race-tiles.xlsx
+++ b/Tile-race-tiles.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="206">
   <si>
     <t>tile</t>
   </si>
@@ -35,7 +35,7 @@
     <t>Vorkath Head</t>
   </si>
   <si>
-    <t>One Head from Vorkath</t>
+    <t>Head from Vorkath</t>
   </si>
   <si>
     <t>vorkath_head.png</t>
@@ -59,7 +59,7 @@
     <t>DT2 Unique</t>
   </si>
   <si>
-    <t>Two DT2 unique from any boss (ingot, quarts or 2x orb)</t>
+    <t>Two DT2 unique from any boss (ingot, quarts, virtus, pet or 2x orb)</t>
   </si>
   <si>
     <t>Virtus_robe.png</t>
@@ -71,7 +71,7 @@
     <t>2 DKs ring</t>
   </si>
   <si>
-    <t>Two rings from any of the DKs no ring of life</t>
+    <t>Two rings from any of the DKs (no ring of life)</t>
   </si>
   <si>
     <t>Berserker_ring.png</t>
@@ -83,7 +83,7 @@
     <t>GoTR</t>
   </si>
   <si>
-    <t>Any of the following items from guardians of the rift (both needles, catalytic, dyes, lantern and pet)</t>
+    <t>Any of the following items from guardians of the rift: Both needles, catalytic, dyes, lantern, pouch and pet</t>
   </si>
   <si>
     <t>Abyssal_protector.png</t>
@@ -92,10 +92,10 @@
     <t>tile5</t>
   </si>
   <si>
-    <t>Herbiar fossil</t>
-  </si>
-  <si>
-    <t>Get Unidentified rare fossil from herbiboar</t>
+    <t>Herbiboar fossil</t>
+  </si>
+  <si>
+    <t>Get Unidentified large fossil from herbiboar</t>
   </si>
   <si>
     <t>Herbiboar.png</t>
@@ -104,13 +104,13 @@
     <t>tile6</t>
   </si>
   <si>
-    <t>Any wildy item</t>
-  </si>
-  <si>
-    <t>Any wildy item (ring, voidwaker piece, pet, weapon attachment, d-pick and d-2hs)</t>
-  </si>
-  <si>
-    <t>void_hilt.png</t>
+    <t>Revs</t>
+  </si>
+  <si>
+    <t>Any col-log from revenants (no ether and bracelet)</t>
+  </si>
+  <si>
+    <t>Craws_bow.png</t>
   </si>
   <si>
     <t>tile7</t>
@@ -143,7 +143,7 @@
     <t>C-log Tempoross</t>
   </si>
   <si>
-    <t>Any item from the collection log of tempoross (no flakes - soaked pages must be hit twice)</t>
+    <t>Any item from the collection log of tempoross (no flakes - soaked pages must be hit twice unless its the x25 dupe drop)</t>
   </si>
   <si>
     <t>Fish_barrel.png</t>
@@ -167,7 +167,7 @@
     <t>Master Speed</t>
   </si>
   <si>
-    <t>6 different master speed times</t>
+    <t>Complete 6 different master speed times and 3 different perfections CA's (no dupes)</t>
   </si>
   <si>
     <t>master_avernic_defender.png</t>
@@ -176,331 +176,310 @@
     <t>tile12</t>
   </si>
   <si>
-    <t>Entry CA's</t>
-  </si>
-  <si>
-    <t>Complete all the entrymode CA's in ToB as a team</t>
-  </si>
-  <si>
-    <t>Avernic_hilt.png</t>
+    <t>Zombie Axe</t>
+  </si>
+  <si>
+    <t>Obtain a Zombie Axe</t>
+  </si>
+  <si>
+    <t>Zombie_axe.png</t>
   </si>
   <si>
     <t>tile13</t>
   </si>
   <si>
-    <t>Perfection</t>
-  </si>
-  <si>
-    <t>Get 3 different perfections CA's</t>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>missing.png</t>
+  </si>
+  <si>
+    <t>tile14</t>
+  </si>
+  <si>
+    <t>GWD Unique</t>
+  </si>
+  <si>
+    <t>Any Unique from any boss (all items on c-log except nihil shard - shard from minion does not count)</t>
+  </si>
+  <si>
+    <t>Zamorak_hilt.png</t>
+  </si>
+  <si>
+    <t>tile15</t>
+  </si>
+  <si>
+    <t>Hybrid Firecapes</t>
+  </si>
+  <si>
+    <t>Complete 3 fire capes using the 3 different styles (melee, ranged, and mage)</t>
+  </si>
+  <si>
+    <t>Fire_cape.png</t>
+  </si>
+  <si>
+    <t>tile16</t>
+  </si>
+  <si>
+    <t>Mole elite/bone</t>
+  </si>
+  <si>
+    <t>Obtain an elite clue or long/curved bone</t>
+  </si>
+  <si>
+    <t>Giant_mole.png</t>
+  </si>
+  <si>
+    <t>tile17</t>
+  </si>
+  <si>
+    <t>Dragon item KQ</t>
+  </si>
+  <si>
+    <t>Obtain any dragon item from Kalphite Queen (including rare drop table)</t>
+  </si>
+  <si>
+    <t>Dragon_Chain.png</t>
+  </si>
+  <si>
+    <t>tile18</t>
+  </si>
+  <si>
+    <t>Roll again</t>
+  </si>
+  <si>
+    <t>dice.png</t>
+  </si>
+  <si>
+    <t>tile19</t>
+  </si>
+  <si>
+    <t>Trimmed items</t>
+  </si>
+  <si>
+    <t>Get any trimmed plate armour (g) and (t) (any clue type with trimmed armor is acceptable)</t>
+  </si>
+  <si>
+    <t>Adamant_platebody_(g).png</t>
+  </si>
+  <si>
+    <t>tile20</t>
+  </si>
+  <si>
+    <t>Strange lockpick</t>
+  </si>
+  <si>
+    <t>Get 2 strange old lockpicks</t>
+  </si>
+  <si>
+    <t>Strange_lockpick.png</t>
+  </si>
+  <si>
+    <t>tile21</t>
+  </si>
+  <si>
+    <t>CoX unique</t>
+  </si>
+  <si>
+    <t>Any C-log item from cox (this includes dark relic, torn prayerscroll but no capes)</t>
+  </si>
+  <si>
+    <t>elder_maul.png</t>
+  </si>
+  <si>
+    <t>tile22</t>
+  </si>
+  <si>
+    <t>Vials</t>
+  </si>
+  <si>
+    <t>Obtain Vials of blood (noramal, entry and hardmore is acceptalbe)</t>
+  </si>
+  <si>
+    <t>Vial_of_blood.png</t>
+  </si>
+  <si>
+    <t>tile23</t>
+  </si>
+  <si>
+    <t>ToA C-log</t>
+  </si>
+  <si>
+    <t>Get any unique (no kits) from toa</t>
+  </si>
+  <si>
+    <t>Osmumten_fang.png</t>
+  </si>
+  <si>
+    <t>tile24</t>
+  </si>
+  <si>
+    <t>3m+ in materials</t>
+  </si>
+  <si>
+    <t>Get 3m+ from zalcano in the price checker only from the materials droptable</t>
+  </si>
+  <si>
+    <t>Smolcano.png</t>
+  </si>
+  <si>
+    <t>tile25</t>
+  </si>
+  <si>
+    <t>Slayer Unique</t>
+  </si>
+  <si>
+    <t>Get a unique drop from any slayer boss (dust from GG etc. does not count)</t>
+  </si>
+  <si>
+    <t>prim_crystal.png</t>
+  </si>
+  <si>
+    <t>tile26</t>
+  </si>
+  <si>
+    <t>Tzhaar</t>
+  </si>
+  <si>
+    <t>Get unique from Tzhaar (obsidian, shield or maul)</t>
+  </si>
+  <si>
+    <t>Obsidian_platebody.png</t>
+  </si>
+  <si>
+    <t>tile27</t>
+  </si>
+  <si>
+    <t>KBD heads</t>
+  </si>
+  <si>
+    <t>Obtain KBD heads</t>
+  </si>
+  <si>
+    <t>Kbd_heads.png</t>
+  </si>
+  <si>
+    <t>tile28</t>
+  </si>
+  <si>
+    <t>Gauntlet seed</t>
+  </si>
+  <si>
+    <t>Any seed from the gauntlet (weapon, armour, enhanced)</t>
+  </si>
+  <si>
+    <t>enhanced_crystal_weapon_seed.png</t>
+  </si>
+  <si>
+    <t>tile29</t>
+  </si>
+  <si>
+    <t>DT2 world tour</t>
+  </si>
+  <si>
+    <t>C-log item from each boss (vestige, virtus, orb, quarts, pet or ingot)</t>
+  </si>
+  <si>
+    <t>ultor.png</t>
+  </si>
+  <si>
+    <t>tile30</t>
+  </si>
+  <si>
+    <t>LMS</t>
+  </si>
+  <si>
+    <t>Obtain 30 LMS points as a team</t>
+  </si>
+  <si>
+    <t>LMS.png</t>
+  </si>
+  <si>
+    <t>tile31</t>
+  </si>
+  <si>
+    <t>Sarachnis Cudgel</t>
+  </si>
+  <si>
+    <t>Obtain cudgel from sarachnis (pet and jar also completes)</t>
+  </si>
+  <si>
+    <t>Sarachnis_cudgel.png</t>
+  </si>
+  <si>
+    <t>tile32</t>
+  </si>
+  <si>
+    <t>Raid c-log</t>
+  </si>
+  <si>
+    <t>Get any c-log item from raids (no masori assembler kit or KC capes)</t>
+  </si>
+  <si>
+    <t>masori_mask.png</t>
+  </si>
+  <si>
+    <t>tile33</t>
+  </si>
+  <si>
+    <t>Wildy shield</t>
+  </si>
+  <si>
+    <t>Get 3 wildy shield pieces (dupes are allowed)</t>
+  </si>
+  <si>
+    <t>Odium_shard_2.png</t>
+  </si>
+  <si>
+    <t>tile34</t>
+  </si>
+  <si>
+    <t>Wrath vorkath</t>
+  </si>
+  <si>
+    <t>Obtain 3 wrath talismans from Vorkath</t>
+  </si>
+  <si>
+    <t>Wrath_talisman.png</t>
+  </si>
+  <si>
+    <t>tile35</t>
+  </si>
+  <si>
+    <t>Ancient icon</t>
+  </si>
+  <si>
+    <t>Obtain ancient icon from muspah</t>
+  </si>
+  <si>
+    <t>Ancient_icon.png</t>
+  </si>
+  <si>
+    <t>tile36</t>
+  </si>
+  <si>
+    <t>Deathless raider</t>
+  </si>
+  <si>
+    <t>Complete a deathless CM raid (Immortal raid team), 350 ToA with no deaths (Something of an expert myself) and ToB</t>
   </si>
   <si>
     <t>lucky_penny.png</t>
   </si>
   <si>
-    <t>tile14</t>
-  </si>
-  <si>
-    <t>GWD Unique</t>
-  </si>
-  <si>
-    <t>Any Unique from any boss (all items on c-log)</t>
-  </si>
-  <si>
-    <t>Zamorak_hilt.png</t>
-  </si>
-  <si>
-    <t>tile15</t>
-  </si>
-  <si>
-    <t>Hybrid Firecapes</t>
-  </si>
-  <si>
-    <t>Complete 3 fire capes using the 3 different styles melee, ranged, and mage)</t>
-  </si>
-  <si>
-    <t>Fire_cape.png</t>
-  </si>
-  <si>
-    <t>tile16</t>
-  </si>
-  <si>
-    <t>Mole elite/bone</t>
-  </si>
-  <si>
-    <t>Obtain an elite clue or long/curved bone</t>
-  </si>
-  <si>
-    <t>Giant_mole.png</t>
-  </si>
-  <si>
-    <t>tile17</t>
-  </si>
-  <si>
-    <t>Dragon item KQ</t>
-  </si>
-  <si>
-    <t>Obtain any dragon item from KQ table (including rare drop table)</t>
-  </si>
-  <si>
-    <t>Dragon_Chain.png</t>
-  </si>
-  <si>
-    <t>tile18</t>
-  </si>
-  <si>
-    <t>Roll again</t>
-  </si>
-  <si>
-    <t>dice.png</t>
-  </si>
-  <si>
-    <t>tile19</t>
-  </si>
-  <si>
-    <t>Trimmed items</t>
-  </si>
-  <si>
-    <t>Get any trimmed plate armour (g) and (t)</t>
-  </si>
-  <si>
-    <t>Adamant_platebody_(g).png</t>
-  </si>
-  <si>
-    <t>tile20</t>
-  </si>
-  <si>
-    <t>Strange lockpick</t>
-  </si>
-  <si>
-    <t>Get 2 strange old lockpicks</t>
-  </si>
-  <si>
-    <t>Strange_lockpick.png</t>
-  </si>
-  <si>
-    <t>tile21</t>
-  </si>
-  <si>
-    <t>Abyssal whip</t>
-  </si>
-  <si>
-    <t>Obtain an abyssal whip</t>
-  </si>
-  <si>
-    <t>abyssal_whip.png</t>
-  </si>
-  <si>
-    <t>tile22</t>
-  </si>
-  <si>
-    <t>Dark bow</t>
-  </si>
-  <si>
-    <t>Obtain a dark bow</t>
-  </si>
-  <si>
-    <t>Dark_bow.png</t>
-  </si>
-  <si>
-    <t>tile23</t>
-  </si>
-  <si>
-    <t>Elder chaos</t>
-  </si>
-  <si>
-    <t>Get one piece of elder chaos robes</t>
-  </si>
-  <si>
-    <t>Elder_chaos_top.png</t>
-  </si>
-  <si>
-    <t>tile24</t>
-  </si>
-  <si>
-    <t>3m+ in materials</t>
-  </si>
-  <si>
-    <t>Get 3m+ in the price checker only from the materials droptable</t>
-  </si>
-  <si>
-    <t>Smolcano.png</t>
-  </si>
-  <si>
-    <t>tile25</t>
-  </si>
-  <si>
-    <t>Slayer Unique</t>
-  </si>
-  <si>
-    <t>Get a unique drop from any slayer boss (dust from GG etc. does not count)</t>
-  </si>
-  <si>
-    <t>prim_crystal.png</t>
-  </si>
-  <si>
-    <t>tile26</t>
-  </si>
-  <si>
-    <t>Tzhaar</t>
-  </si>
-  <si>
-    <t>Get unique from Tzhaar (obsidian, shield or maul)</t>
-  </si>
-  <si>
-    <t>Obsidian_platebody.png</t>
-  </si>
-  <si>
-    <t>tile27</t>
-  </si>
-  <si>
-    <t>KBD heads</t>
-  </si>
-  <si>
-    <t>Get KBD head from king black dragon</t>
-  </si>
-  <si>
-    <t>Kbd_heads.png</t>
-  </si>
-  <si>
-    <t>tile28</t>
-  </si>
-  <si>
-    <t>Gauntlet seed</t>
-  </si>
-  <si>
-    <t>Any seed from the gauntlet (weapon, armour, enhanced)</t>
-  </si>
-  <si>
-    <t>enhanced_crystal_weapon_seed.png</t>
-  </si>
-  <si>
-    <t>tile29</t>
-  </si>
-  <si>
-    <t>DT2 world tour</t>
-  </si>
-  <si>
-    <t>C-log item from each boss (vestige, virtus, orb or ingot)</t>
-  </si>
-  <si>
-    <t>ultor.png</t>
-  </si>
-  <si>
-    <t>tile30</t>
-  </si>
-  <si>
-    <t>Zenyte</t>
-  </si>
-  <si>
-    <t>Obtain one zenyte</t>
-  </si>
-  <si>
-    <t>zenyte.png</t>
-  </si>
-  <si>
-    <t>tile31</t>
-  </si>
-  <si>
-    <t>Sarachnis Cudgel</t>
-  </si>
-  <si>
-    <t>Obtain cudgel from sarachnis</t>
-  </si>
-  <si>
-    <t>Sarachnis_cudgel.png</t>
-  </si>
-  <si>
-    <t>tile32</t>
-  </si>
-  <si>
-    <t>Raid c-log</t>
-  </si>
-  <si>
-    <t>Get any c-log item from raids (no masori assembler kit)</t>
-  </si>
-  <si>
-    <t>masori_mask.png</t>
-  </si>
-  <si>
-    <t>tile33</t>
-  </si>
-  <si>
-    <t>Wildy shield</t>
-  </si>
-  <si>
-    <t>Get 3 wildy shield pieces (dupes are allowed)</t>
-  </si>
-  <si>
-    <t>Odium_shard_2.png</t>
-  </si>
-  <si>
-    <t>tile34</t>
-  </si>
-  <si>
-    <t>Onyx Vorkath</t>
-  </si>
-  <si>
-    <t>Obtain onyx bolt tips from vorkath</t>
-  </si>
-  <si>
-    <t>Onyx_bolt_tips.png</t>
-  </si>
-  <si>
-    <t>tile35</t>
-  </si>
-  <si>
-    <t>Ancient icon</t>
-  </si>
-  <si>
-    <t>Obtain ancient icon from muspah</t>
-  </si>
-  <si>
-    <t>Ancient_icon.png</t>
-  </si>
-  <si>
-    <t>tile36</t>
-  </si>
-  <si>
-    <t>Deathless CM</t>
-  </si>
-  <si>
-    <t>Complete a deathless challengemode chambers of xeric (Immortal raid team)</t>
-  </si>
-  <si>
-    <t>Metamorphic_dust.png</t>
-  </si>
-  <si>
     <t>tile37</t>
   </si>
   <si>
-    <t>ToA Expert</t>
-  </si>
-  <si>
-    <t>Complete a 350 ToA with no deaths (Something of an expert myself)</t>
-  </si>
-  <si>
-    <t>Tumeken.png</t>
-  </si>
-  <si>
     <t>tile38</t>
   </si>
   <si>
-    <t>Any ToB?</t>
-  </si>
-  <si>
-    <t>Complete a ToB run with 2 perfect room achievements</t>
-  </si>
-  <si>
-    <t>Scythe_of_vitur.png</t>
-  </si>
-  <si>
     <t>tile39</t>
   </si>
   <si>
-    <t>Nightmare coins</t>
-  </si>
-  <si>
-    <t>Get coin drop from nightmare or phosani (normal nightmare needs 2 coin drops)</t>
+    <t>Phosani</t>
+  </si>
+  <si>
+    <t>Get runes drop 5 times from Phosani</t>
   </si>
   <si>
     <t>Inquisitor_hauberk.png</t>
@@ -509,13 +488,13 @@
     <t>tile40</t>
   </si>
   <si>
-    <t>Any jars</t>
-  </si>
-  <si>
-    <t>Get any jar in the game</t>
-  </si>
-  <si>
-    <t>Jar_of_eyes.png</t>
+    <t>Scurrius</t>
+  </si>
+  <si>
+    <t>Get 5x Scurrius' spine</t>
+  </si>
+  <si>
+    <t>Scurrius.png</t>
   </si>
   <si>
     <t>tile41</t>
@@ -524,13 +503,13 @@
     <t>tile42</t>
   </si>
   <si>
-    <t>Spirit seed</t>
-  </si>
-  <si>
-    <t>Obtain a spirit seed</t>
-  </si>
-  <si>
-    <t>Spirit_seed.png</t>
+    <t>Easy Clues</t>
+  </si>
+  <si>
+    <t>Obtain any elegant item or any bob shirt</t>
+  </si>
+  <si>
+    <t>Bob_shirt.png</t>
   </si>
   <si>
     <t>tile43</t>
@@ -539,7 +518,7 @@
     <t>Common GWD</t>
   </si>
   <si>
-    <t>Get any of zammy spear, steam bstaff, sara sword or sara light</t>
+    <t>Get any of: Zamorakian Spear, Steam Battlestaff, Saradomin Sword, or Saradomin's light</t>
   </si>
   <si>
     <t>Zamorakian_spear.png</t>
@@ -551,7 +530,7 @@
     <t>Nex item</t>
   </si>
   <si>
-    <t>Get any unique nex item or 600 Nihil shards as a team</t>
+    <t>Get any unique nex item or 150 Nihil shards as a team</t>
   </si>
   <si>
     <t>Torva_platebody_(damaged).png</t>
@@ -563,7 +542,7 @@
     <t>Wildy item</t>
   </si>
   <si>
-    <t>Wildy item (ring, voidwaker piece, pet, weapon attachment)</t>
+    <t>Any wildy item (rings, voidwaker piece, pet, or weapon attachment)</t>
   </si>
   <si>
     <t>ring_of_gods.png</t>
@@ -596,13 +575,13 @@
     <t>tile48</t>
   </si>
   <si>
-    <t>ToA purple</t>
-  </si>
-  <si>
-    <t>Obtain a purple from tombs of amascus</t>
-  </si>
-  <si>
-    <t>Osmumten_fang.png</t>
+    <t>Clue hunter</t>
+  </si>
+  <si>
+    <t>Complete 5 elite or master clues (no imps, keys or skotizo)</t>
+  </si>
+  <si>
+    <t>elite_clue.png</t>
   </si>
   <si>
     <t>tile49</t>
@@ -944,10 +923,10 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="2" width="18.0"/>
-    <col customWidth="1" min="3" max="3" width="87.29"/>
+    <col customWidth="1" min="3" max="3" width="101.71"/>
     <col customWidth="1" min="4" max="4" width="32.57"/>
     <col customWidth="1" min="5" max="5" width="8.43"/>
-    <col customWidth="1" min="6" max="25" width="8.71"/>
+    <col customWidth="1" min="6" max="22" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -974,7 +953,7 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1008,7 +987,7 @@
       <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -1025,7 +1004,7 @@
       <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -1042,7 +1021,7 @@
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -1073,13 +1052,13 @@
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>32</v>
       </c>
       <c r="E8" s="3" t="b">
@@ -1120,7 +1099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" ht="15.0" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>41</v>
       </c>
@@ -1161,14 +1140,14 @@
       <c r="B13" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>52</v>
       </c>
       <c r="E13" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -1185,7 +1164,7 @@
         <v>56</v>
       </c>
       <c r="E14" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1196,10 +1175,10 @@
         <v>58</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="E15" s="3" t="b">
         <v>0</v>
@@ -1207,16 +1186,16 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="E16" s="3" t="b">
         <v>0</v>
@@ -1224,33 +1203,33 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="3" t="b">
+      <c r="E17" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="E18" s="3" t="b">
         <v>0</v>
@@ -1258,16 +1237,16 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="E19" s="3" t="b">
         <v>0</v>
@@ -1275,16 +1254,16 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="E20" s="3" t="b">
         <v>0</v>
@@ -1292,16 +1271,16 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="E21" s="3" t="b">
         <v>0</v>
@@ -1309,33 +1288,33 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" ht="15.0" customHeight="1">
+      <c r="A23" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E22" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="2" t="s">
+      <c r="B23" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="E23" s="3" t="b">
         <v>0</v>
@@ -1343,16 +1322,16 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>95</v>
       </c>
       <c r="E24" s="3" t="b">
         <v>0</v>
@@ -1360,16 +1339,16 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="E25" s="4" t="b">
         <v>0</v>
@@ -1377,16 +1356,16 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="C26" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="E26" s="3" t="b">
         <v>0</v>
@@ -1394,16 +1373,16 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="D27" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="E27" s="4" t="b">
         <v>0</v>
@@ -1411,16 +1390,16 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>111</v>
       </c>
       <c r="E28" s="4" t="b">
         <v>0</v>
@@ -1428,16 +1407,16 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="E29" s="4" t="b">
         <v>0</v>
@@ -1445,16 +1424,16 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>119</v>
       </c>
       <c r="E30" s="4" t="b">
         <v>0</v>
@@ -1462,16 +1441,16 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="E31" s="4" t="b">
         <v>0</v>
@@ -1479,16 +1458,16 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>126</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>127</v>
       </c>
       <c r="E32" s="4" t="b">
         <v>0</v>
@@ -1496,16 +1475,16 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="C33" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="D33" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="E33" s="4" t="b">
         <v>0</v>
@@ -1513,16 +1492,16 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="C34" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="D34" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>135</v>
       </c>
       <c r="E34" s="4" t="b">
         <v>1</v>
@@ -1530,16 +1509,16 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="C35" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="D35" s="4" t="s">
         <v>138</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>139</v>
       </c>
       <c r="E35" s="4" t="b">
         <v>0</v>
@@ -1547,16 +1526,16 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="D36" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>143</v>
       </c>
       <c r="E36" s="3" t="b">
         <v>0</v>
@@ -1564,16 +1543,16 @@
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="D37" s="4" t="s">
         <v>146</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>147</v>
       </c>
       <c r="E37" s="3" t="b">
         <v>0</v>
@@ -1581,16 +1560,16 @@
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="D38" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>151</v>
       </c>
       <c r="E38" s="3" t="b">
         <v>0</v>
@@ -1598,16 +1577,16 @@
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>153</v>
+        <v>58</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>154</v>
+        <v>58</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>155</v>
+        <v>59</v>
       </c>
       <c r="E39" s="3" t="b">
         <v>0</v>
@@ -1615,16 +1594,16 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>158</v>
+        <v>58</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="E40" s="4" t="b">
         <v>0</v>
@@ -1632,16 +1611,16 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="E41" s="3" t="b">
         <v>0</v>
@@ -1649,16 +1628,16 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="2" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E42" s="4" t="b">
         <v>0</v>
@@ -1666,16 +1645,16 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B43" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="E43" s="3" t="b">
         <v>0</v>
@@ -1683,16 +1662,16 @@
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="2" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E44" s="3" t="b">
         <v>0</v>
@@ -1700,16 +1679,16 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="2" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E45" s="3" t="b">
         <v>0</v>
@@ -1717,16 +1696,16 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="2" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E46" s="3" t="b">
         <v>0</v>
@@ -1734,16 +1713,16 @@
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="2" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="E47" s="4" t="b">
         <v>0</v>
@@ -1751,16 +1730,16 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="2" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="E48" s="4" t="b">
         <v>0</v>
@@ -1768,16 +1747,16 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="2" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="E49" s="3" t="b">
         <v>0</v>
@@ -1785,16 +1764,16 @@
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="2" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="E50" s="3" t="b">
         <v>0</v>
@@ -1802,16 +1781,16 @@
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E51" s="3" t="b">
         <v>0</v>
@@ -1819,16 +1798,16 @@
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="2" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="E52" s="3" t="b">
         <v>0</v>
@@ -1836,16 +1815,16 @@
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="2" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="E53" s="4" t="b">
         <v>1</v>
@@ -1853,16 +1832,16 @@
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="2" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="E54" s="4" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Updated board from Excel
</commit_message>
<xml_diff>
--- a/Tile-race-tiles.xlsx
+++ b/Tile-race-tiles.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="217">
   <si>
     <t>tile</t>
   </si>
@@ -188,10 +188,13 @@
     <t>tile13</t>
   </si>
   <si>
-    <t>Missing</t>
-  </si>
-  <si>
-    <t>missing.png</t>
+    <t>Elder chaos</t>
+  </si>
+  <si>
+    <t>Obtain a pieve of elder chaos robes</t>
+  </si>
+  <si>
+    <t>Elder_chaos_top.png</t>
   </si>
   <si>
     <t>tile14</t>
@@ -245,10 +248,13 @@
     <t>tile18</t>
   </si>
   <si>
-    <t>Roll again</t>
-  </si>
-  <si>
-    <t>dice.png</t>
+    <t>Blood shard</t>
+  </si>
+  <si>
+    <t>Obtain a blood shard</t>
+  </si>
+  <si>
+    <t>Blood_shard.png</t>
   </si>
   <si>
     <t>tile19</t>
@@ -437,7 +443,7 @@
     <t>Wrath vorkath</t>
   </si>
   <si>
-    <t>Obtain 3 wrath talismans from Vorkath</t>
+    <t>Obtain 5 wrath talismans from Vorkath</t>
   </si>
   <si>
     <t>Wrath_talisman.png</t>
@@ -461,7 +467,7 @@
     <t>Deathless raider</t>
   </si>
   <si>
-    <t>Complete a deathless CM raid (Immortal raid team), 350 ToA with no deaths (Something of an expert myself) and ToB</t>
+    <t>Complete a deathless CM raid (Immortal raid team) and 350 ToA with no deaths (Something of an expert myself)</t>
   </si>
   <si>
     <t>lucky_penny.png</t>
@@ -470,9 +476,27 @@
     <t>tile37</t>
   </si>
   <si>
+    <t>Champion scroll</t>
+  </si>
+  <si>
+    <t>Obtain any champion scroll</t>
+  </si>
+  <si>
+    <t>champion_scroll.png</t>
+  </si>
+  <si>
     <t>tile38</t>
   </si>
   <si>
+    <t>Chaos ely</t>
+  </si>
+  <si>
+    <t>Get pet or dragon pickaxe from chaos elemental</t>
+  </si>
+  <si>
+    <t>Dragon_pick.png</t>
+  </si>
+  <si>
     <t>tile39</t>
   </si>
   <si>
@@ -500,6 +524,15 @@
     <t>tile41</t>
   </si>
   <si>
+    <t>Common GWD</t>
+  </si>
+  <si>
+    <t>Get any of: Zamorakian Spear, Steam Battlestaff, Saradomin Sword, or Saradomin's light</t>
+  </si>
+  <si>
+    <t>Zamorakian_spear.png</t>
+  </si>
+  <si>
     <t>tile42</t>
   </si>
   <si>
@@ -515,13 +548,13 @@
     <t>tile43</t>
   </si>
   <si>
-    <t>Common GWD</t>
-  </si>
-  <si>
-    <t>Get any of: Zamorakian Spear, Steam Battlestaff, Saradomin Sword, or Saradomin's light</t>
-  </si>
-  <si>
-    <t>Zamorakian_spear.png</t>
+    <t>Zulrah fang</t>
+  </si>
+  <si>
+    <t>Get a fang item from Zulrah (Magic Fang or Tanzanite fang)</t>
+  </si>
+  <si>
+    <t>magic_fang.png</t>
   </si>
   <si>
     <t>tile44</t>
@@ -563,13 +596,13 @@
     <t>tile47</t>
   </si>
   <si>
-    <t>Zulrah fang</t>
-  </si>
-  <si>
-    <t>Get a fang item from Zulrah (Magic Fang or Tanzanite fang)</t>
-  </si>
-  <si>
-    <t>magic_fang.png</t>
+    <t>GWD armor</t>
+  </si>
+  <si>
+    <t>Obtain a armor piece from GWD (bandos boots, chest and plate + arma chest, legs and helm)</t>
+  </si>
+  <si>
+    <t>Arma_chest.png</t>
   </si>
   <si>
     <t>tile48</t>
@@ -688,7 +721,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -701,6 +734,9 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1175,10 +1211,10 @@
         <v>58</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E15" s="3" t="b">
         <v>0</v>
@@ -1186,16 +1222,16 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E16" s="3" t="b">
         <v>0</v>
@@ -1203,16 +1239,16 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E17" s="4" t="b">
         <v>0</v>
@@ -1220,16 +1256,16 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E18" s="3" t="b">
         <v>0</v>
@@ -1237,16 +1273,16 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E19" s="3" t="b">
         <v>0</v>
@@ -1254,16 +1290,16 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E20" s="3" t="b">
         <v>0</v>
@@ -1271,16 +1307,16 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E21" s="3" t="b">
         <v>0</v>
@@ -1288,16 +1324,16 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E22" s="4" t="b">
         <v>0</v>
@@ -1305,16 +1341,16 @@
     </row>
     <row r="23" ht="15.0" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E23" s="3" t="b">
         <v>0</v>
@@ -1322,16 +1358,16 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E24" s="3" t="b">
         <v>0</v>
@@ -1339,16 +1375,16 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E25" s="4" t="b">
         <v>0</v>
@@ -1356,16 +1392,16 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E26" s="3" t="b">
         <v>0</v>
@@ -1373,16 +1409,16 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E27" s="4" t="b">
         <v>0</v>
@@ -1390,16 +1426,16 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E28" s="4" t="b">
         <v>0</v>
@@ -1407,16 +1443,16 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E29" s="4" t="b">
         <v>0</v>
@@ -1424,16 +1460,16 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E30" s="4" t="b">
         <v>0</v>
@@ -1441,16 +1477,16 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E31" s="4" t="b">
         <v>0</v>
@@ -1458,16 +1494,16 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E32" s="4" t="b">
         <v>0</v>
@@ -1475,16 +1511,16 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E33" s="4" t="b">
         <v>0</v>
@@ -1492,33 +1528,33 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E34" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E35" s="4" t="b">
         <v>0</v>
@@ -1526,16 +1562,16 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E36" s="3" t="b">
         <v>0</v>
@@ -1543,16 +1579,16 @@
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E37" s="3" t="b">
         <v>0</v>
@@ -1560,33 +1596,33 @@
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="E38" s="3" t="b">
-        <v>0</v>
+        <v>152</v>
+      </c>
+      <c r="E38" s="4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>58</v>
+        <v>155</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>59</v>
+        <v>156</v>
       </c>
       <c r="E39" s="3" t="b">
         <v>0</v>
@@ -1594,16 +1630,16 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="2" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>58</v>
+        <v>158</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>58</v>
+        <v>159</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>59</v>
+        <v>160</v>
       </c>
       <c r="E40" s="4" t="b">
         <v>0</v>
@@ -1611,16 +1647,16 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="E41" s="3" t="b">
         <v>0</v>
@@ -1628,33 +1664,33 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="2" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="E42" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="2" t="s">
-        <v>161</v>
+      <c r="A43" s="5" t="s">
+        <v>169</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>77</v>
+        <v>170</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>77</v>
+        <v>171</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>78</v>
+        <v>172</v>
       </c>
       <c r="E43" s="3" t="b">
         <v>0</v>
@@ -1662,33 +1698,33 @@
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="2" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="E44" s="3" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="2" t="s">
-        <v>166</v>
+      <c r="A45" s="5" t="s">
+        <v>177</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>169</v>
+        <v>179</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="E45" s="3" t="b">
         <v>0</v>
@@ -1696,16 +1732,16 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="2" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="E46" s="3" t="b">
         <v>0</v>
@@ -1713,16 +1749,16 @@
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="2" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="E47" s="4" t="b">
         <v>0</v>
@@ -1730,16 +1766,16 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="2" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="E48" s="4" t="b">
         <v>0</v>
@@ -1747,16 +1783,16 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="2" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>185</v>
+        <v>195</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>196</v>
       </c>
       <c r="E49" s="3" t="b">
         <v>0</v>
@@ -1764,16 +1800,16 @@
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="2" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="E50" s="3" t="b">
         <v>0</v>
@@ -1781,16 +1817,16 @@
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="2" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="E51" s="3" t="b">
         <v>0</v>
@@ -1798,16 +1834,16 @@
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="2" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="E52" s="3" t="b">
         <v>0</v>
@@ -1815,16 +1851,16 @@
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="2" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="E53" s="4" t="b">
         <v>1</v>
@@ -1832,16 +1868,16 @@
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="2" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
       <c r="E54" s="4" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Changed board and added yew seed picture
</commit_message>
<xml_diff>
--- a/Tile-race-tiles.xlsx
+++ b/Tile-race-tiles.xlsx
@@ -248,13 +248,13 @@
     <t>tile18</t>
   </si>
   <si>
-    <t>Blood shard</t>
-  </si>
-  <si>
-    <t>Obtain a blood shard</t>
-  </si>
-  <si>
-    <t>Blood_shard.png</t>
+    <t>Scurrius</t>
+  </si>
+  <si>
+    <t>Get 5x Scurrius' spine</t>
+  </si>
+  <si>
+    <t>Scurrius.png</t>
   </si>
   <si>
     <t>tile19</t>
@@ -287,7 +287,7 @@
     <t>CoX unique</t>
   </si>
   <si>
-    <t>Any C-log item from cox (this includes dark relic, torn prayerscroll but no capes)</t>
+    <t>Unique item from cox  (torn prayerscroll counts)</t>
   </si>
   <si>
     <t>elder_maul.png</t>
@@ -311,7 +311,7 @@
     <t>ToA C-log</t>
   </si>
   <si>
-    <t>Get any unique (no kits) from toa</t>
+    <t>Get any unique (no kits no chest) from toa</t>
   </si>
   <si>
     <t>Osmumten_fang.png</t>
@@ -512,13 +512,13 @@
     <t>tile40</t>
   </si>
   <si>
-    <t>Scurrius</t>
-  </si>
-  <si>
-    <t>Get 5x Scurrius' spine</t>
-  </si>
-  <si>
-    <t>Scurrius.png</t>
+    <t>Vorkath Yew seed</t>
+  </si>
+  <si>
+    <t>Obtain a Yew seed from Vorkath</t>
+  </si>
+  <si>
+    <t>Yew_seed.png</t>
   </si>
   <si>
     <t>tile41</t>
@@ -623,7 +623,7 @@
     <t>Venator shard</t>
   </si>
   <si>
-    <t>Obtain a venator shard</t>
+    <t>Obtain two venator shards</t>
   </si>
   <si>
     <t>Venator_shard.png</t>
@@ -1288,8 +1288,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="2" t="s">
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="5" t="s">
         <v>77</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -1301,7 +1301,7 @@
       <c r="D20" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E20" s="3" t="b">
+      <c r="E20" s="4" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1662,8 +1662,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="2" t="s">
+    <row r="42">
+      <c r="A42" s="5" t="s">
         <v>165</v>
       </c>
       <c r="B42" s="4" t="s">
@@ -1675,7 +1675,7 @@
       <c r="D42" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="E42" s="4" t="b">
+      <c r="E42" s="3" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1822,7 +1822,7 @@
       <c r="B51" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="4" t="s">
         <v>203</v>
       </c>
       <c r="D51" s="3" t="s">

</xml_diff>